<commit_message>
úprava K2 bez výstupu
</commit_message>
<xml_diff>
--- a/vystupy/struktura_Tabulek.xlsx
+++ b/vystupy/struktura_Tabulek.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lokalni_data_mimo_OD\K2\vystupy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5421B6E-AEAE-4E21-9E6C-B089D50215C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2055F3C9-AD0B-429F-93AA-C18CE3B7DB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4185" yWindow="3255" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="K2_MIGUSER1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">K2_MIGUSER1!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>TABLE_NAME</t>
   </si>
@@ -31,6 +34,9 @@
     <t>ROW_COUNT</t>
   </si>
   <si>
+    <t>ARE_CUSTOMER_CHECK</t>
+  </si>
+  <si>
     <t>LX_CRMT_CUSTOMER_RELATEDCUSTOMERS_IDITEMS</t>
   </si>
   <si>
@@ -52,15 +58,174 @@
     <t>L0_ARES_VR_STATUTARNI_ORGANY</t>
   </si>
   <si>
+    <t>L0_CATT_ENT_CATALOG</t>
+  </si>
+  <si>
+    <t>L0_CATT_ENT_CATALOG_CATEGORY</t>
+  </si>
+  <si>
+    <t>L0_CATT_ENT_CATALOG_SPEC</t>
+  </si>
+  <si>
+    <t>L0_CATT_ENT_CATALOG_SPEC_REL</t>
+  </si>
+  <si>
+    <t>L0_CATT_ENT_CATALOG_SPEC_REL_TYPE</t>
+  </si>
+  <si>
+    <t>L0_CATT_ENT_CATALOG_SPEC_STATUS</t>
+  </si>
+  <si>
+    <t>L0_CATT_ENT_CATALOG_SPEC_TYPE</t>
+  </si>
+  <si>
+    <t>L0_CATT_ENT_CATALOG_STATUS</t>
+  </si>
+  <si>
+    <t>L0_CATT_PRICE_LIST</t>
+  </si>
+  <si>
+    <t>L0_CNFT_ENTITY_SPECIFICATION</t>
+  </si>
+  <si>
+    <t>L0_CNFT_REGISTER</t>
+  </si>
+  <si>
+    <t>L0_CNFT_REGISTER_VALUE</t>
+  </si>
+  <si>
+    <t>L0_CRMT_ACCOUNT</t>
+  </si>
+  <si>
+    <t>L0_CRMT_ACCOUNT_TYPE</t>
+  </si>
+  <si>
+    <t>L0_CRMT_CRM_ADDRESS</t>
+  </si>
+  <si>
+    <t>L0_CRMT_CRM_ADDRESS_ROLE</t>
+  </si>
+  <si>
+    <t>L0_CRMT_CRM_ADDRESS_ROLE_TYPE</t>
+  </si>
+  <si>
+    <t>L0_CRMT_CUSTOMER</t>
+  </si>
+  <si>
+    <t>L0_CRMT_CUSTOMER_LEGAL_FORM</t>
+  </si>
+  <si>
+    <t>L0_CRMT_CUSTOMER_SEGMENT</t>
+  </si>
+  <si>
+    <t>L0_CRMT_CUSTOMER_TYPE</t>
+  </si>
+  <si>
+    <t>L0_CRMT_PERSON</t>
+  </si>
+  <si>
+    <t>L0_CRMT_PERSON_ROLE</t>
+  </si>
+  <si>
+    <t>L0_CRMT_PERSON_ROLE_ACCOUNT</t>
+  </si>
+  <si>
+    <t>L0_CRMT_PERSON_ROLE_TYPE</t>
+  </si>
+  <si>
+    <t>L0_CRMT_PERSON_TYPE</t>
+  </si>
+  <si>
+    <t>L0_INVT_ENT_INST</t>
+  </si>
+  <si>
+    <t>L0_INVT_ENT_INST_CONF</t>
+  </si>
+  <si>
+    <t>L0_INVT_ENT_INST_CONF_REL</t>
+  </si>
+  <si>
+    <t>L0_INVT_ENT_INST_CONF_STATUS</t>
+  </si>
+  <si>
     <t>L0_PREVAL_CUSTOMER</t>
   </si>
   <si>
+    <t>L0_TICT_CATEGORY</t>
+  </si>
+  <si>
+    <t>L0_TICT_STATUS</t>
+  </si>
+  <si>
+    <t>L0_TICT_TYPE</t>
+  </si>
+  <si>
+    <t>L1_CUSTOMER_CHECK</t>
+  </si>
+  <si>
+    <t>L1_CUSTOMER_CHECK_VALIDATION</t>
+  </si>
+  <si>
+    <t>L1_K2_CUSTOMER_CHECK_300</t>
+  </si>
+  <si>
+    <t>L1_MSA_ACCOUNT</t>
+  </si>
+  <si>
+    <t>L1_MSA_CORE_PRODUCT</t>
+  </si>
+  <si>
+    <t>L1_MSA_CP</t>
+  </si>
+  <si>
+    <t>L1_MSA_CUSTOMER</t>
+  </si>
+  <si>
+    <t>L1_MSA_PRODUCTS</t>
+  </si>
+  <si>
+    <t>L1_MSA_TARIF</t>
+  </si>
+  <si>
+    <t>L1_TE_ACCOUNT</t>
+  </si>
+  <si>
+    <t>L1_TE_CUSTOMER</t>
+  </si>
+  <si>
+    <t>L1_TE_PERSON</t>
+  </si>
+  <si>
+    <t>L1_TE_PRODUCT</t>
+  </si>
+  <si>
+    <t>L1_TE_VALIDATION</t>
+  </si>
+  <si>
     <t>MSA_CONFIG</t>
   </si>
   <si>
+    <t>MSA_DQ_VAL_BAD_ROWS_LIST</t>
+  </si>
+  <si>
     <t>MSA_LOG</t>
   </si>
   <si>
+    <t>MSA_METADATA</t>
+  </si>
+  <si>
+    <t>MSA_VAL_BAD_ROWS_LIST</t>
+  </si>
+  <si>
+    <t>MSA_VAL_DESIGN</t>
+  </si>
+  <si>
+    <t>MSA_VALIDATIONS</t>
+  </si>
+  <si>
+    <t>MSA_VAL_TABLES_USED_IN_WAVE</t>
+  </si>
+  <si>
     <t>REP_FO</t>
   </si>
   <si>
@@ -79,9 +244,18 @@
     <t>TE_TREE</t>
   </si>
   <si>
+    <t>TE_TREE_LOG</t>
+  </si>
+  <si>
     <t>TE_TREE_PLUGIN_LOG</t>
   </si>
   <si>
+    <t>TE_TREE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>TMP_JTO_ALL_SERVICES</t>
+  </si>
+  <si>
     <t>TMP_JTO_TV_ONLY</t>
   </si>
   <si>
@@ -97,6 +271,9 @@
     <t>TMP_JTO_TV_ONLY_RC</t>
   </si>
   <si>
+    <t>Obsah ESLUZBA, PM_LINE, a vygenerovane O2 produkty pro zakaznika</t>
+  </si>
+  <si>
     <t>table of tree edges - edge to destination (node_to) can be added to path if value returned by plugin from source (from_node) meets defined condition - CDR rating engine rating tree configuration</t>
   </si>
   <si>
@@ -107,6 +284,9 @@
   </si>
   <si>
     <t>tree table</t>
+  </si>
+  <si>
+    <t>Prirazuje jednotlive stromy ke konkretnim entitam. Strom se spusti v zadany cas.</t>
   </si>
 </sst>
 </file>
@@ -474,18 +654,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A23"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="68.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="48.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -503,7 +678,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>2621</v>
+        <v>79634</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -511,7 +686,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -519,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -527,7 +702,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>8766</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -535,7 +710,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>8648</v>
+        <v>9010</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -543,7 +718,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>15950</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -551,7 +726,7 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>7014</v>
+        <v>16465</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -559,7 +734,7 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>7199</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -567,7 +742,7 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -575,7 +750,7 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>1035</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -583,7 +758,7 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>17</v>
+        <v>9472</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,51 +766,39 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>133</v>
+        <v>9235</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
       <c r="C14">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
       <c r="C15">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
       <c r="C16">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
       <c r="C17">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -643,7 +806,7 @@
         <v>19</v>
       </c>
       <c r="C18">
-        <v>837</v>
+        <v>3112</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -651,7 +814,7 @@
         <v>20</v>
       </c>
       <c r="C19">
-        <v>2765</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -659,7 +822,7 @@
         <v>21</v>
       </c>
       <c r="C20">
-        <v>1533</v>
+        <v>334</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -667,7 +830,7 @@
         <v>22</v>
       </c>
       <c r="C21">
-        <v>61</v>
+        <v>364553</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -675,7 +838,7 @@
         <v>23</v>
       </c>
       <c r="C22">
-        <v>890</v>
+        <v>114779</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -683,10 +846,485 @@
         <v>24</v>
       </c>
       <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>380144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>1315034</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>114778</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <v>153957</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32">
+        <v>171293</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36">
+        <v>810138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37">
+        <v>1243848</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38">
+        <v>256848</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62">
+        <v>5294</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>68</v>
+      </c>
+      <c r="C67">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" t="s">
+        <v>83</v>
+      </c>
+      <c r="C68">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" t="s">
+        <v>84</v>
+      </c>
+      <c r="C69">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70" t="s">
+        <v>85</v>
+      </c>
+      <c r="C70">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" t="s">
+        <v>86</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>73</v>
+      </c>
+      <c r="C72">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" t="s">
+        <v>87</v>
+      </c>
+      <c r="C74">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>76</v>
+      </c>
+      <c r="C75">
+        <v>79004</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76">
+        <v>2765</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>78</v>
+      </c>
+      <c r="C77">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>79</v>
+      </c>
+      <c r="C78">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>80</v>
+      </c>
+      <c r="C79">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80">
         <v>593</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>